<commit_message>
in report export consider measures in different programs use same sub measures, new template for report export
</commit_message>
<xml_diff>
--- a/src/app/client/report/Asset Management Customer Value 2021 - UK Template.xlsx
+++ b/src/app/client/report/Asset Management Customer Value 2021 - UK Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iProject\upmark_check\Upmark\src\app\client\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67090CB2-BE3C-4DF2-845D-710F05EB2D2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4EAD44-2421-467C-9EFA-A8AD02E47B52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="2850" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMCV Analysis" sheetId="1" r:id="rId1"/>
@@ -7904,9 +7904,7 @@
         <f t="array" ref="P3">IF(O3=2,O3+MEDIAN(IF($B$3:$B$981=L3,IF($D$3:$D$981=3,$I$3:$I$789))),O3)</f>
         <v>2.5</v>
       </c>
-      <c r="Q3" s="32">
-        <v>0.75</v>
-      </c>
+      <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
       <c r="S3" s="42">
         <f t="shared" ref="S3:S41" si="2">IF(P3&gt;=2.75,IF(Q3&gt;=0.75,P3+Q3+R3,P3+Q3),P3)</f>
@@ -8020,9 +8018,7 @@
         <f t="array" ref="P5">IF(O5=2,O5+MEDIAN(IF($B$3:$B$981=L5,IF($D$3:$D$981=3,$I$3:$I$789))),O5)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="32">
-        <v>0.75</v>
-      </c>
+      <c r="Q5" s="32"/>
       <c r="R5" s="32"/>
       <c r="S5" s="42">
         <f t="shared" si="2"/>
@@ -8250,9 +8246,7 @@
         <f t="array" ref="P9">IF(O9=2,O9+MEDIAN(IF($B$3:$B$981=L9,IF($D$3:$D$981=3,$I$3:$I$789))),O9)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="32">
-        <v>0.5</v>
-      </c>
+      <c r="Q9" s="32"/>
       <c r="R9" s="32"/>
       <c r="S9" s="42">
         <f t="shared" si="2"/>
@@ -8309,12 +8303,8 @@
         <f t="array" ref="P10">IF(O10=2,O10+MEDIAN(IF($B$3:$B$981=L10,IF($D$3:$D$981=3,$I$3:$I$789))),O10)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="32">
-        <v>0.75</v>
-      </c>
-      <c r="R10" s="32">
-        <v>1</v>
-      </c>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
       <c r="S10" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -23452,4 +23442,404 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Topic xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xsi:nil="true"/>
+    <Theme xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xsi:nil="true"/>
+    <NetworkOwner xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xsi:nil="true"/>
+    <WSAAportal xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </WSAAportal>
+    <TaxCatchAll xmlns="e9c2f33e-1257-44b0-9f12-8b9d4d157a10" xsi:nil="true"/>
+    <YearCompleted xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xsi:nil="true"/>
+    <Foldertype xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xsi:nil="true"/>
+    <Year xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xsi:nil="true"/>
+    <e4d1394bb46240aea058fa24384ac488 xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e4d1394bb46240aea058fa24384ac488>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C2D3FA73E183B249B8CE315F540D0D7B" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f334f393eb7af5dd2384490be8f624e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xmlns:ns3="e9c2f33e-1257-44b0-9f12-8b9d4d157a10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17c003db29046d1580156d55247efba3" ns2:_="" ns3:_="">
+    <xsd:import namespace="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe"/>
+    <xsd:import namespace="e9c2f33e-1257-44b0-9f12-8b9d4d157a10"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:Year" minOccurs="0"/>
+                <xsd:element ref="ns2:YearCompleted" minOccurs="0"/>
+                <xsd:element ref="ns2:Topic" minOccurs="0"/>
+                <xsd:element ref="ns2:NetworkOwner" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:WSAAportal" minOccurs="0"/>
+                <xsd:element ref="ns2:e4d1394bb46240aea058fa24384ac488" minOccurs="0"/>
+                <xsd:element ref="ns2:Theme" minOccurs="0"/>
+                <xsd:element ref="ns2:Foldertype" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Year" ma:index="21" nillable="true" ma:displayName="Year" ma:format="Dropdown" ma:internalName="Year">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="2019"/>
+          <xsd:enumeration value="2020"/>
+          <xsd:enumeration value="2021"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="YearCompleted" ma:index="22" nillable="true" ma:displayName="Year Completed" ma:format="Dropdown" ma:internalName="YearCompleted">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="2017"/>
+          <xsd:enumeration value="2018"/>
+          <xsd:enumeration value="2019"/>
+          <xsd:enumeration value="2020"/>
+          <xsd:enumeration value="2021"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Topic" ma:index="23" nillable="true" ma:displayName="Topic" ma:format="Dropdown" ma:internalName="Topic">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Training"/>
+          <xsd:enumeration value="Codes"/>
+          <xsd:enumeration value="Bulk Water"/>
+          <xsd:enumeration value="Chemicals"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NetworkOwner" ma:index="24" nillable="true" ma:displayName="Network Owner" ma:format="Dropdown" ma:internalName="NetworkOwner">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="James Goode"/>
+          <xsd:enumeration value="Peter Gee"/>
+          <xsd:enumeration value="Greg Ryan"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="WSAAportal" ma:index="26" nillable="true" ma:displayName="WSAA portal" ma:format="Hyperlink" ma:internalName="WSAAportal">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="e4d1394bb46240aea058fa24384ac488" ma:index="28" nillable="true" ma:taxonomy="true" ma:internalName="e4d1394bb46240aea058fa24384ac488" ma:taxonomyFieldName="Owner" ma:displayName="Owner" ma:indexed="true" ma:default="" ma:fieldId="{e4d1394b-b462-40ae-a058-fa24384ac488}" ma:sspId="1702b5c8-0a88-4fca-a898-27150c795514" ma:termSetId="fc5e52b8-9005-4fa8-9f96-3973b9b0eb62" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Theme" ma:index="29" nillable="true" ma:displayName="Theme" ma:format="Dropdown" ma:internalName="Theme">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoice">
+            <xsd:sequence>
+              <xsd:element name="Value" maxOccurs="unbounded" minOccurs="0" nillable="true">
+                <xsd:simpleType>
+                  <xsd:restriction base="dms:Choice">
+                    <xsd:enumeration value="Water Tanks"/>
+                    <xsd:enumeration value="Condition Assessment - Water"/>
+                    <xsd:enumeration value="Condition Assessment - Sewer"/>
+                    <xsd:enumeration value="Water Quality"/>
+                    <xsd:enumeration value="Sewage"/>
+                    <xsd:enumeration value="Decision Making"/>
+                    <xsd:enumeration value="Business case"/>
+                  </xsd:restriction>
+                </xsd:simpleType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Foldertype" ma:index="30" nillable="true" ma:displayName="Folder type" ma:format="Dropdown" ma:internalName="Foldertype">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Administration"/>
+          <xsd:enumeration value="Meeting"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e9c2f33e-1257-44b0-9f12-8b9d4d157a10" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="25" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{d1fe3237-90a3-4f17-8afa-b55e5c28c35a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="e9c2f33e-1257-44b0-9f12-8b9d4d157a10">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8EA6C9-4C24-422C-84F5-A03553A51A32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe"/>
+    <ds:schemaRef ds:uri="e9c2f33e-1257-44b0-9f12-8b9d4d157a10"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF23E37F-91D3-4031-BE1F-4260D9D8C853}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe"/>
+    <ds:schemaRef ds:uri="e9c2f33e-1257-44b0-9f12-8b9d4d157a10"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1013150-F71E-4BC5-81BA-504989332191}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
report template for survey "Asset Management Customer Value 2021 - UK"
</commit_message>
<xml_diff>
--- a/src/app/client/report/Asset Management Customer Value 2021 - UK Template.xlsx
+++ b/src/app/client/report/Asset Management Customer Value 2021 - UK Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iProject\upmark_check\Upmark\src\app\client\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4EAD44-2421-467C-9EFA-A8AD02E47B52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD018043-E7D5-4118-82BB-C0C8CC13C9B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="2850" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMCV Analysis" sheetId="1" r:id="rId1"/>
@@ -6407,6 +6407,9 @@
                 <c:pt idx="201">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="202">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="203">
                   <c:v>0</c:v>
                 </c:pt>
@@ -7415,15 +7418,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>50165</xdr:colOff>
+      <xdr:colOff>46990</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>20319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>69215</xdr:colOff>
+      <xdr:colOff>66040</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>372745</xdr:rowOff>
+      <xdr:rowOff>369570</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7451,9 +7454,9 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>602886</xdr:colOff>
+      <xdr:colOff>599711</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>352697</xdr:rowOff>
+      <xdr:rowOff>349522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
@@ -7753,7 +7756,7 @@
   <dimension ref="A1:T698"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
@@ -14462,7 +14465,9 @@
       <c r="G185" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="H185" s="25"/>
+      <c r="H185" s="25">
+        <v>0</v>
+      </c>
       <c r="I185" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -15069,8 +15074,13 @@
       <c r="G205" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="H205" s="25"/>
-      <c r="I205" s="21"/>
+      <c r="H205" s="25">
+        <v>0</v>
+      </c>
+      <c r="I205" s="25">
+        <f t="shared" ref="I205" si="18">H205/4</f>
+        <v>0</v>
+      </c>
       <c r="L205" s="9"/>
       <c r="M205" s="43"/>
     </row>
@@ -15220,7 +15230,7 @@
         <v>0</v>
       </c>
       <c r="I210" s="25">
-        <f t="shared" ref="I210:I217" si="18">H210/4</f>
+        <f t="shared" ref="I210:I217" si="19">H210/4</f>
         <v>0</v>
       </c>
     </row>
@@ -15250,7 +15260,7 @@
         <v>0</v>
       </c>
       <c r="I211" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -15280,7 +15290,7 @@
         <v>0</v>
       </c>
       <c r="I212" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -15310,7 +15320,7 @@
         <v>0</v>
       </c>
       <c r="I213" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -15340,7 +15350,7 @@
         <v>0</v>
       </c>
       <c r="I214" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -15370,7 +15380,7 @@
         <v>0</v>
       </c>
       <c r="I215" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -15400,7 +15410,7 @@
         <v>0</v>
       </c>
       <c r="I216" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -15430,7 +15440,7 @@
         <v>0</v>
       </c>
       <c r="I217" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -15587,7 +15597,7 @@
         <v>0</v>
       </c>
       <c r="I222" s="25">
-        <f t="shared" ref="I222:I227" si="19">H222/4</f>
+        <f t="shared" ref="I222:I227" si="20">H222/4</f>
         <v>0</v>
       </c>
     </row>
@@ -15617,7 +15627,7 @@
         <v>0</v>
       </c>
       <c r="I223" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -15647,7 +15657,7 @@
         <v>0</v>
       </c>
       <c r="I224" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -15677,7 +15687,7 @@
         <v>0</v>
       </c>
       <c r="I225" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -15707,7 +15717,7 @@
         <v>0</v>
       </c>
       <c r="I226" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -15737,7 +15747,7 @@
         <v>0</v>
       </c>
       <c r="I227" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -15887,7 +15897,7 @@
         <v>0</v>
       </c>
       <c r="I232" s="25">
-        <f t="shared" ref="I232:I240" si="20">H232/4</f>
+        <f t="shared" ref="I232:I240" si="21">H232/4</f>
         <v>0</v>
       </c>
     </row>
@@ -15917,7 +15927,7 @@
         <v>0</v>
       </c>
       <c r="I233" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -15947,7 +15957,7 @@
         <v>0</v>
       </c>
       <c r="I234" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -15977,7 +15987,7 @@
         <v>0</v>
       </c>
       <c r="I235" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -16007,7 +16017,7 @@
         <v>0</v>
       </c>
       <c r="I236" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -16037,7 +16047,7 @@
         <v>0</v>
       </c>
       <c r="I237" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -16067,7 +16077,7 @@
         <v>0</v>
       </c>
       <c r="I238" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -16097,7 +16107,7 @@
         <v>0</v>
       </c>
       <c r="I239" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="N239" s="1"/>
@@ -16134,7 +16144,7 @@
         <v>0</v>
       </c>
       <c r="I240" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -16284,7 +16294,7 @@
         <v>0</v>
       </c>
       <c r="I245" s="25">
-        <f t="shared" ref="I245:I250" si="21">H245/4</f>
+        <f t="shared" ref="I245:I250" si="22">H245/4</f>
         <v>0</v>
       </c>
     </row>
@@ -16314,7 +16324,7 @@
         <v>0</v>
       </c>
       <c r="I246" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -16344,7 +16354,7 @@
         <v>0</v>
       </c>
       <c r="I247" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -16374,7 +16384,7 @@
         <v>0</v>
       </c>
       <c r="I248" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L248" s="9"/>
@@ -16406,7 +16416,7 @@
         <v>0</v>
       </c>
       <c r="I249" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -16436,7 +16446,7 @@
         <v>0</v>
       </c>
       <c r="I250" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -16586,7 +16596,7 @@
         <v>0</v>
       </c>
       <c r="I255" s="25">
-        <f t="shared" ref="I255:I262" si="22">H255/4</f>
+        <f t="shared" ref="I255:I262" si="23">H255/4</f>
         <v>0</v>
       </c>
     </row>
@@ -16616,7 +16626,7 @@
         <v>0</v>
       </c>
       <c r="I256" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -16646,7 +16656,7 @@
         <v>0</v>
       </c>
       <c r="I257" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N257" s="1"/>
@@ -16683,7 +16693,7 @@
         <v>0</v>
       </c>
       <c r="I258" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L258" s="9"/>
@@ -16715,7 +16725,7 @@
         <v>0</v>
       </c>
       <c r="I259" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -16745,7 +16755,7 @@
         <v>0</v>
       </c>
       <c r="I260" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -16775,7 +16785,7 @@
         <v>0</v>
       </c>
       <c r="I261" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -16805,7 +16815,7 @@
         <v>0</v>
       </c>
       <c r="I262" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -16955,7 +16965,7 @@
         <v>0</v>
       </c>
       <c r="I267" s="25">
-        <f t="shared" ref="I267:I272" si="23">H267/4</f>
+        <f t="shared" ref="I267:I272" si="24">H267/4</f>
         <v>0</v>
       </c>
     </row>
@@ -16985,7 +16995,7 @@
         <v>0</v>
       </c>
       <c r="I268" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L268" s="9"/>
@@ -17017,7 +17027,7 @@
         <v>0</v>
       </c>
       <c r="I269" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -17047,7 +17057,7 @@
         <v>0</v>
       </c>
       <c r="I270" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -17077,7 +17087,7 @@
         <v>0</v>
       </c>
       <c r="I271" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -17107,7 +17117,7 @@
         <v>0</v>
       </c>
       <c r="I272" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -17264,7 +17274,7 @@
         <v>0</v>
       </c>
       <c r="I277" s="25">
-        <f t="shared" ref="I277:I282" si="24">H277/4</f>
+        <f t="shared" ref="I277:I282" si="25">H277/4</f>
         <v>0</v>
       </c>
     </row>
@@ -17294,7 +17304,7 @@
         <v>0</v>
       </c>
       <c r="I278" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -17324,7 +17334,7 @@
         <v>0</v>
       </c>
       <c r="I279" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="L279" s="9"/>
@@ -17356,7 +17366,7 @@
         <v>0</v>
       </c>
       <c r="I280" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -17386,7 +17396,7 @@
         <v>0</v>
       </c>
       <c r="I281" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -17416,7 +17426,7 @@
         <v>0</v>
       </c>
       <c r="I282" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -17566,7 +17576,7 @@
         <v>3</v>
       </c>
       <c r="I287" s="25">
-        <f t="shared" ref="I287:I296" si="25">H287/4</f>
+        <f t="shared" ref="I287:I296" si="26">H287/4</f>
         <v>0.75</v>
       </c>
     </row>
@@ -17596,7 +17606,7 @@
         <v>3</v>
       </c>
       <c r="I288" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
     </row>
@@ -17626,7 +17636,7 @@
         <v>3</v>
       </c>
       <c r="I289" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
     </row>
@@ -17656,7 +17666,7 @@
         <v>3</v>
       </c>
       <c r="I290" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
     </row>
@@ -17686,7 +17696,7 @@
         <v>3</v>
       </c>
       <c r="I291" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
     </row>
@@ -17716,7 +17726,7 @@
         <v>3</v>
       </c>
       <c r="I292" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
     </row>
@@ -17746,7 +17756,7 @@
         <v>3</v>
       </c>
       <c r="I293" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
       <c r="N293" s="1"/>
@@ -17783,7 +17793,7 @@
         <v>3</v>
       </c>
       <c r="I294" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
     </row>
@@ -17813,7 +17823,7 @@
         <v>3</v>
       </c>
       <c r="I295" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
     </row>
@@ -17843,13 +17853,10 @@
         <v>3</v>
       </c>
       <c r="I296" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
-      <c r="J296">
-        <f>MEDIAN(I287:I296)</f>
-        <v>0.75</v>
-      </c>
+      <c r="J296"/>
     </row>
     <row r="297" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="10" t="s">
@@ -17997,7 +18004,7 @@
         <v>0</v>
       </c>
       <c r="I301" s="25">
-        <f t="shared" ref="I301:I312" si="26">H301/4</f>
+        <f t="shared" ref="I301:I312" si="27">H301/4</f>
         <v>0</v>
       </c>
     </row>
@@ -18027,7 +18034,7 @@
         <v>0</v>
       </c>
       <c r="I302" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18057,7 +18064,7 @@
         <v>0</v>
       </c>
       <c r="I303" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L303" s="9"/>
@@ -18089,7 +18096,7 @@
         <v>0</v>
       </c>
       <c r="I304" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18119,7 +18126,7 @@
         <v>0</v>
       </c>
       <c r="I305" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18149,7 +18156,7 @@
         <v>0</v>
       </c>
       <c r="I306" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18179,7 +18186,7 @@
         <v>0</v>
       </c>
       <c r="I307" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18209,7 +18216,7 @@
         <v>0</v>
       </c>
       <c r="I308" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J308" s="1"/>
@@ -18240,7 +18247,7 @@
         <v>0</v>
       </c>
       <c r="I309" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18270,7 +18277,7 @@
         <v>0</v>
       </c>
       <c r="I310" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18300,7 +18307,7 @@
         <v>0</v>
       </c>
       <c r="I311" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N311" s="1"/>
@@ -18337,7 +18344,7 @@
         <v>0</v>
       </c>
       <c r="I312" s="25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -18487,7 +18494,7 @@
         <v>0</v>
       </c>
       <c r="I317" s="25">
-        <f t="shared" ref="I317:I329" si="27">H317/4</f>
+        <f t="shared" ref="I317:I329" si="28">H317/4</f>
         <v>0</v>
       </c>
       <c r="J317" s="1"/>
@@ -18518,7 +18525,7 @@
         <v>0</v>
       </c>
       <c r="I318" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18548,7 +18555,7 @@
         <v>0</v>
       </c>
       <c r="I319" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18578,7 +18585,7 @@
         <v>0</v>
       </c>
       <c r="I320" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18608,7 +18615,7 @@
         <v>0</v>
       </c>
       <c r="I321" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18638,7 +18645,7 @@
         <v>0</v>
       </c>
       <c r="I322" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18668,7 +18675,7 @@
         <v>0</v>
       </c>
       <c r="I323" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18698,7 +18705,7 @@
         <v>0</v>
       </c>
       <c r="I324" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18728,7 +18735,7 @@
         <v>0</v>
       </c>
       <c r="I325" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18758,7 +18765,7 @@
         <v>0</v>
       </c>
       <c r="I326" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18788,7 +18795,7 @@
         <v>0</v>
       </c>
       <c r="I327" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18818,7 +18825,7 @@
         <v>0</v>
       </c>
       <c r="I328" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18848,7 +18855,7 @@
         <v>0</v>
       </c>
       <c r="I329" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -18998,7 +19005,7 @@
         <v>0</v>
       </c>
       <c r="I334" s="25">
-        <f t="shared" ref="I334:I344" si="28">H334/4</f>
+        <f t="shared" ref="I334:I344" si="29">H334/4</f>
         <v>0</v>
       </c>
     </row>
@@ -19028,7 +19035,7 @@
         <v>0</v>
       </c>
       <c r="I335" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19058,7 +19065,7 @@
         <v>0</v>
       </c>
       <c r="I336" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19088,7 +19095,7 @@
         <v>0</v>
       </c>
       <c r="I337" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19118,7 +19125,7 @@
         <v>0</v>
       </c>
       <c r="I338" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19148,7 +19155,7 @@
         <v>0</v>
       </c>
       <c r="I339" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19178,7 +19185,7 @@
         <v>0</v>
       </c>
       <c r="I340" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19208,7 +19215,7 @@
         <v>0</v>
       </c>
       <c r="I341" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L341" s="9"/>
@@ -19240,7 +19247,7 @@
         <v>0</v>
       </c>
       <c r="I342" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19270,7 +19277,7 @@
         <v>0</v>
       </c>
       <c r="I343" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19300,7 +19307,7 @@
         <v>0</v>
       </c>
       <c r="I344" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -19457,7 +19464,7 @@
         <v>2</v>
       </c>
       <c r="I349" s="25">
-        <f t="shared" ref="I349:I360" si="29">H349/4</f>
+        <f t="shared" ref="I349:I360" si="30">H349/4</f>
         <v>0.5</v>
       </c>
     </row>
@@ -19487,7 +19494,7 @@
         <v>2</v>
       </c>
       <c r="I350" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19517,7 +19524,7 @@
         <v>2</v>
       </c>
       <c r="I351" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19547,7 +19554,7 @@
         <v>2</v>
       </c>
       <c r="I352" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19577,7 +19584,7 @@
         <v>2</v>
       </c>
       <c r="I353" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19607,7 +19614,7 @@
         <v>2</v>
       </c>
       <c r="I354" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19637,7 +19644,7 @@
         <v>2</v>
       </c>
       <c r="I355" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19667,7 +19674,7 @@
         <v>2</v>
       </c>
       <c r="I356" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19697,7 +19704,7 @@
         <v>2</v>
       </c>
       <c r="I357" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
       <c r="L357" s="9"/>
@@ -19729,7 +19736,7 @@
         <v>2</v>
       </c>
       <c r="I358" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19759,7 +19766,7 @@
         <v>2</v>
       </c>
       <c r="I359" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19789,7 +19796,7 @@
         <v>2</v>
       </c>
       <c r="I360" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
     </row>
@@ -19939,7 +19946,7 @@
         <v>0</v>
       </c>
       <c r="I365" s="25">
-        <f t="shared" ref="I365:I373" si="30">H365/4</f>
+        <f t="shared" ref="I365:I373" si="31">H365/4</f>
         <v>0</v>
       </c>
     </row>
@@ -19969,7 +19976,7 @@
         <v>0</v>
       </c>
       <c r="I366" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="L366" s="9"/>
@@ -20001,7 +20008,7 @@
         <v>0</v>
       </c>
       <c r="I367" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -20031,7 +20038,7 @@
         <v>0</v>
       </c>
       <c r="I368" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -20061,7 +20068,7 @@
         <v>0</v>
       </c>
       <c r="I369" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -20091,7 +20098,7 @@
         <v>0</v>
       </c>
       <c r="I370" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -20121,7 +20128,7 @@
         <v>0</v>
       </c>
       <c r="I371" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="J371" s="1"/>
@@ -20152,7 +20159,7 @@
         <v>0</v>
       </c>
       <c r="I372" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -20182,7 +20189,7 @@
         <v>0</v>
       </c>
       <c r="I373" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -20332,7 +20339,7 @@
         <v>0</v>
       </c>
       <c r="I378" s="25">
-        <f t="shared" ref="I378:I390" si="31">H378/4</f>
+        <f t="shared" ref="I378:I390" si="32">H378/4</f>
         <v>0</v>
       </c>
     </row>
@@ -20362,7 +20369,7 @@
         <v>0</v>
       </c>
       <c r="I379" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20392,7 +20399,7 @@
         <v>0</v>
       </c>
       <c r="I380" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20422,7 +20429,7 @@
         <v>0</v>
       </c>
       <c r="I381" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20452,7 +20459,7 @@
         <v>0</v>
       </c>
       <c r="I382" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20482,7 +20489,7 @@
         <v>0</v>
       </c>
       <c r="I383" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20512,7 +20519,7 @@
         <v>0</v>
       </c>
       <c r="I384" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N384" s="1"/>
@@ -20549,7 +20556,7 @@
         <v>0</v>
       </c>
       <c r="I385" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20579,7 +20586,7 @@
         <v>0</v>
       </c>
       <c r="I386" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20609,7 +20616,7 @@
         <v>0</v>
       </c>
       <c r="I387" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20639,7 +20646,7 @@
         <v>0</v>
       </c>
       <c r="I388" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20669,7 +20676,7 @@
         <v>0</v>
       </c>
       <c r="I389" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20699,7 +20706,7 @@
         <v>0</v>
       </c>
       <c r="I390" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20850,7 +20857,7 @@
         <v>0</v>
       </c>
       <c r="I395" s="25">
-        <f t="shared" ref="I395:I401" si="32">H395/4</f>
+        <f t="shared" ref="I395:I401" si="33">H395/4</f>
         <v>0</v>
       </c>
     </row>
@@ -20880,7 +20887,7 @@
         <v>0</v>
       </c>
       <c r="I396" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -20910,7 +20917,7 @@
         <v>0</v>
       </c>
       <c r="I397" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -20940,7 +20947,7 @@
         <v>0</v>
       </c>
       <c r="I398" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -20970,7 +20977,7 @@
         <v>0</v>
       </c>
       <c r="I399" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -21000,7 +21007,7 @@
         <v>0</v>
       </c>
       <c r="I400" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -21030,7 +21037,7 @@
         <v>0</v>
       </c>
       <c r="I401" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -21399,7 +21406,7 @@
         <v>4</v>
       </c>
       <c r="I413" s="25">
-        <f t="shared" ref="I413:I418" si="33">H413/4</f>
+        <f t="shared" ref="I413:I418" si="34">H413/4</f>
         <v>1</v>
       </c>
     </row>
@@ -21429,7 +21436,7 @@
         <v>4</v>
       </c>
       <c r="I414" s="25">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
     </row>
@@ -21459,7 +21466,7 @@
         <v>4</v>
       </c>
       <c r="I415" s="25">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="J415" s="1"/>
@@ -21490,7 +21497,7 @@
         <v>4</v>
       </c>
       <c r="I416" s="25">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
     </row>
@@ -21520,7 +21527,7 @@
         <v>4</v>
       </c>
       <c r="I417" s="25">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
     </row>
@@ -21550,7 +21557,7 @@
         <v>4</v>
       </c>
       <c r="I418" s="25">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
     </row>
@@ -21709,7 +21716,7 @@
         <v>0</v>
       </c>
       <c r="I423" s="25">
-        <f t="shared" ref="I423:I429" si="34">H423/4</f>
+        <f t="shared" ref="I423:I429" si="35">H423/4</f>
         <v>0</v>
       </c>
     </row>
@@ -21739,7 +21746,7 @@
         <v>0</v>
       </c>
       <c r="I424" s="25">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J424" s="1"/>
@@ -21770,7 +21777,7 @@
         <v>0</v>
       </c>
       <c r="I425" s="25">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -21800,7 +21807,7 @@
         <v>0</v>
       </c>
       <c r="I426" s="25">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -21830,7 +21837,7 @@
         <v>0</v>
       </c>
       <c r="I427" s="25">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -21860,7 +21867,7 @@
         <v>0</v>
       </c>
       <c r="I428" s="25">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -21890,7 +21897,7 @@
         <v>0</v>
       </c>
       <c r="I429" s="25">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -22040,7 +22047,7 @@
         <v>0</v>
       </c>
       <c r="I434" s="25">
-        <f t="shared" ref="I434:I440" si="35">H434/4</f>
+        <f t="shared" ref="I434:I440" si="36">H434/4</f>
         <v>0</v>
       </c>
     </row>
@@ -22070,7 +22077,7 @@
         <v>0</v>
       </c>
       <c r="I435" s="25">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -22100,7 +22107,7 @@
         <v>0</v>
       </c>
       <c r="I436" s="25">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -22130,7 +22137,7 @@
         <v>0</v>
       </c>
       <c r="I437" s="25">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -22160,7 +22167,7 @@
         <v>0</v>
       </c>
       <c r="I438" s="25">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -22190,7 +22197,7 @@
         <v>0</v>
       </c>
       <c r="I439" s="25">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -22220,7 +22227,7 @@
         <v>0</v>
       </c>
       <c r="I440" s="25">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -22377,7 +22384,7 @@
         <v>0</v>
       </c>
       <c r="I445" s="25">
-        <f t="shared" ref="I445:I452" si="36">H445/4</f>
+        <f t="shared" ref="I445:I452" si="37">H445/4</f>
         <v>0</v>
       </c>
     </row>
@@ -22407,7 +22414,7 @@
         <v>0</v>
       </c>
       <c r="I446" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -22437,7 +22444,7 @@
         <v>0</v>
       </c>
       <c r="I447" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -22467,7 +22474,7 @@
         <v>0</v>
       </c>
       <c r="I448" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -22497,7 +22504,7 @@
         <v>0</v>
       </c>
       <c r="I449" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -22527,7 +22534,7 @@
         <v>0</v>
       </c>
       <c r="I450" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -22557,7 +22564,7 @@
         <v>0</v>
       </c>
       <c r="I451" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -22587,7 +22594,7 @@
         <v>0</v>
       </c>
       <c r="I452" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -22737,7 +22744,7 @@
         <v>0</v>
       </c>
       <c r="I457" s="25">
-        <f t="shared" ref="I457:I463" si="37">H457/4</f>
+        <f t="shared" ref="I457:I463" si="38">H457/4</f>
         <v>0</v>
       </c>
     </row>
@@ -22767,7 +22774,7 @@
         <v>0</v>
       </c>
       <c r="I458" s="25">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -22797,7 +22804,7 @@
         <v>0</v>
       </c>
       <c r="I459" s="25">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -22827,7 +22834,7 @@
         <v>0</v>
       </c>
       <c r="I460" s="25">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -22857,7 +22864,7 @@
         <v>0</v>
       </c>
       <c r="I461" s="25">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="N461" s="1"/>
@@ -22894,7 +22901,7 @@
         <v>0</v>
       </c>
       <c r="I462" s="25">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -22924,7 +22931,7 @@
         <v>0</v>
       </c>
       <c r="I463" s="25">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -23445,6 +23452,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Topic xmlns="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xsi:nil="true"/>
@@ -23465,7 +23481,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C2D3FA73E183B249B8CE315F540D0D7B" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f334f393eb7af5dd2384490be8f624e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe" xmlns:ns3="e9c2f33e-1257-44b0-9f12-8b9d4d157a10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17c003db29046d1580156d55247efba3" ns2:_="" ns3:_="">
     <xsd:import namespace="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe"/>
@@ -23797,27 +23813,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1013150-F71E-4BC5-81BA-504989332191}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8EA6C9-4C24-422C-84F5-A03553A51A32}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eeec6feb-2bb9-4dcc-a56c-824cc5afeafe"/>
     <ds:schemaRef ds:uri="e9c2f33e-1257-44b0-9f12-8b9d4d157a10"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF23E37F-91D3-4031-BE1F-4260D9D8C853}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23834,12 +23855,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1013150-F71E-4BC5-81BA-504989332191}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>